<commit_message>
bot_web_pdf - README em andamento
</commit_message>
<xml_diff>
--- a/bot_pdf_excel/spreadsheet/RelacaoUsuario.xlsx
+++ b/bot_pdf_excel/spreadsheet/RelacaoUsuario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t xml:space="preserve">NOME</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">2022004387@ifam.edu.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021002252@ifam.edu.br</t>
   </si>
 </sst>
 </file>
@@ -72,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,12 +103,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -158,28 +161,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,22 +371,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="30.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -400,8 +399,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -414,8 +413,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -424,12 +423,12 @@
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -438,7 +437,21 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -447,6 +460,7 @@
     <hyperlink ref="C2" r:id="rId1" display="7caioc@gmail.com"/>
     <hyperlink ref="C3" r:id="rId2" display="lucas.andrade@ifam.edu.br"/>
     <hyperlink ref="C4" r:id="rId3" display="2022004387@ifam.edu.br"/>
+    <hyperlink ref="C5" r:id="rId4" display="2021002252@ifam.edu.br"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>